<commit_message>
add logic to create TestNg report & Extent Report and  Logger & object properties used into project
</commit_message>
<xml_diff>
--- a/Excel/Data.xlsx
+++ b/Excel/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>userName</t>
   </si>
@@ -27,16 +27,19 @@
   <si>
     <t>P@ssw0rd1@2</t>
   </si>
+  <si>
+    <t>P@ssw0rd1@</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -65,6 +68,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -72,7 +90,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -86,14 +104,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -102,14 +113,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,21 +126,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -154,38 +142,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,31 +203,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,55 +341,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,91 +383,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,17 +397,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -419,21 +418,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -472,6 +456,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -480,164 +494,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -973,7 +976,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1002,12 +1005,12 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1019,8 +1022,8 @@
     <hyperlink ref="A2" r:id="rId1" display="mansukhmayur99@gmail.com"/>
     <hyperlink ref="B2" r:id="rId2" display="P@ssw0rd1@2"/>
     <hyperlink ref="A3" r:id="rId1" display="mansukhmayur99@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="P@ssw0rd1@2" tooltip="mailto:P@ssw0rd1@2"/>
-    <hyperlink ref="A4" r:id="rId1" display="mansukhmayur99@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="P@ssw0rd1@" tooltip="mailto:P@ssw0rd1@"/>
+    <hyperlink ref="A4" r:id="rId1" display="mansukhmayur99@gmail.com" tooltip="mailto:mansukhmayur99@gmail.com"/>
     <hyperlink ref="B4" r:id="rId2" display="P@ssw0rd1@2" tooltip="mailto:P@ssw0rd1@2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add logic to implement Keyword driven method and upload file method into project
</commit_message>
<xml_diff>
--- a/Excel/Data.xlsx
+++ b/Excel/Data.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>userName</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Action</t>
   </si>
   <si>
     <t>mansukhmayur99@gmail.com</t>
@@ -28,7 +31,13 @@
     <t>P@ssw0rd1@2</t>
   </si>
   <si>
-    <t>P@ssw0rd1@</t>
+    <t xml:space="preserve"> test with data1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test with data2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test with data3</t>
   </si>
 </sst>
 </file>
@@ -36,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -68,6 +77,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -75,7 +91,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -89,43 +142,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -151,7 +167,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,30 +188,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,187 +212,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,17 +403,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -419,6 +417,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,21 +470,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -494,153 +492,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -973,56 +982,69 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="30.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="16.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="mansukhmayur99@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="P@ssw0rd1@2"/>
+    <hyperlink ref="B2" r:id="rId2" display="P@ssw0rd1@2" tooltip="mailto:P@ssw0rd1@2"/>
     <hyperlink ref="A3" r:id="rId1" display="mansukhmayur99@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId3" display="P@ssw0rd1@" tooltip="mailto:P@ssw0rd1@"/>
+    <hyperlink ref="B3" r:id="rId2" display="P@ssw0rd1@2" tooltip="mailto:P@ssw0rd1@2"/>
     <hyperlink ref="A4" r:id="rId1" display="mansukhmayur99@gmail.com" tooltip="mailto:mansukhmayur99@gmail.com"/>
     <hyperlink ref="B4" r:id="rId2" display="P@ssw0rd1@2" tooltip="mailto:P@ssw0rd1@2"/>
   </hyperlinks>

</xml_diff>